<commit_message>
Split screen with a cleaner fmxl file look.  Menu bar items work but buttons not yet implemented.
</commit_message>
<xml_diff>
--- a/testRead.xlsx
+++ b/testRead.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -159,6 +159,18 @@
   </si>
   <si>
     <t>A number of ways of passing data to other scenes and dialogs</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Dealing with "Location not set"</t>
+  </si>
+  <si>
+    <t>https://edencoding.com/location-not-set/</t>
+  </si>
+  <si>
+    <t>Where JavaFX stores .fxml files and other resources</t>
   </si>
 </sst>
 </file>
@@ -209,7 +221,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -409,6 +421,23 @@
         <v>23</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Fully working split screen - Category view button added but not yet implemented
</commit_message>
<xml_diff>
--- a/testRead.xlsx
+++ b/testRead.xlsx
@@ -134,13 +134,13 @@
     <t>https://code.makery.ch/library/javafx-tutorial/part5/</t>
   </si>
   <si>
-    <t>A small JavaFX project but with lots of useful learning - XML, Dialogs</t>
+    <t>A small JavaFX project but with lots of useful learning - XML, Dialogs, and how to package your programme</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>Eden Coding</t>
+    <t>Eden Coding - MVC</t>
   </si>
   <si>
     <t>https://edencoding.com/mvc-in-javafx/</t>
@@ -230,7 +230,7 @@
     <col min="1" max="1" width="3.26953125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="30.68359375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="73.1640625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="61.7578125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="96.39453125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.2265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Working on new CategoryView - Scene switch only
</commit_message>
<xml_diff>
--- a/testRead.xlsx
+++ b/testRead.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -92,7 +92,7 @@
     <t>Barry Greene</t>
   </si>
   <si>
-    <t>www.videos.com</t>
+    <t>https://barrygreenevideolessons.vhx.tv/</t>
   </si>
   <si>
     <t>Jazz Guitar instruction</t>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>Where JavaFX stores .fxml files and other resources</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Creating mobile apps with JavaFX</t>
+  </si>
+  <si>
+    <t>https://foojay.io/today/creating-mobile-apps-with-javafx-part-1/</t>
+  </si>
+  <si>
+    <t>How to run a JavaFX programme on mobiles using Gluon</t>
   </si>
 </sst>
 </file>
@@ -221,14 +233,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="3.26953125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="30.68359375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="30.87890625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="73.1640625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="96.39453125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.2265625" customWidth="true" bestFit="true"/>
@@ -438,6 +450,23 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Most of CategoryView working well - still need to implement edit functions About to switch to Dark Theme (MainView already switched)
</commit_message>
<xml_diff>
--- a/testRead.xlsx
+++ b/testRead.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -183,6 +183,18 @@
   </si>
   <si>
     <t>How to run a JavaFX programme on mobiles using Gluon</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Oracle JavaFX CSS reference</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javafx/2/api/javafx/scene/doc-files/cssref.html</t>
+  </si>
+  <si>
+    <t>A good reference for the JavaFX CSS - including colours, fonts etc.</t>
   </si>
 </sst>
 </file>
@@ -233,7 +245,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -467,6 +479,23 @@
         <v>23</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored to update views via extractor and bindings - more efficient
</commit_message>
<xml_diff>
--- a/testRead.xlsx
+++ b/testRead.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -56,6 +56,21 @@
     <t>British Telecom Website</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Java Docs</t>
+  </si>
+  <si>
+    <t>Oracle.com</t>
+  </si>
+  <si>
+    <t>Java docs</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
@@ -78,9 +93,6 @@
   </si>
   <si>
     <t>A small JavaFX project but with lots of useful learning - XML, Dialogs, and how to package your programme</t>
-  </si>
-  <si>
-    <t>Coding</t>
   </si>
   <si>
     <t>12</t>
@@ -245,7 +257,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -323,24 +335,24 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -357,7 +369,7 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -374,7 +386,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -391,7 +403,7 @@
         <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
@@ -408,7 +420,7 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -425,7 +437,7 @@
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -442,41 +454,41 @@
         <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>51</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>56</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14">
@@ -493,7 +505,24 @@
         <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>